<commit_message>
Changeset to Python data cleaning & analyses
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Python\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -96,12 +96,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -125,8 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,28 +420,28 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -657,5 +667,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>